<commit_message>
feat: new model 5 context improvement
</commit_message>
<xml_diff>
--- a/output/predicted_unlabeled_dataset.xlsx
+++ b/output/predicted_unlabeled_dataset.xlsx
@@ -487,7 +487,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Geografi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -575,7 +575,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -592,7 +592,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -740,7 +740,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -798,7 +798,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -815,7 +815,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -884,7 +884,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Geografi</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -1577,7 +1577,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -2144,7 +2144,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Geografi</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -2507,7 +2507,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -2983,7 +2983,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Geografi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -3622,7 +3622,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -3823,7 +3823,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Geografi</t>
         </is>
       </c>
     </row>
@@ -3934,7 +3934,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -4025,7 +4025,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -4240,7 +4240,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>Geografi</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -4293,7 +4293,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -4706,7 +4706,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -4723,7 +4723,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -4740,7 +4740,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -4780,7 +4780,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -4822,7 +4822,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -4963,7 +4963,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -5239,7 +5239,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -5256,7 +5256,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -5310,7 +5310,7 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -5560,7 +5560,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -5598,7 +5598,7 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -5619,7 +5619,7 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -5658,7 +5658,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -5678,7 +5678,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -5730,7 +5730,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -5802,7 +5802,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -5836,7 +5836,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -5910,7 +5910,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -5930,7 +5930,7 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -5947,7 +5947,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -5982,7 +5982,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -5999,7 +5999,7 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -6039,7 +6039,7 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -6150,7 +6150,7 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -6224,7 +6224,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -6378,7 +6378,7 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -6448,7 +6448,7 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -6466,7 +6466,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -6523,7 +6523,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -6541,7 +6541,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -6559,7 +6559,7 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -6681,7 +6681,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -6866,7 +6866,7 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -6948,7 +6948,7 @@
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -6969,7 +6969,7 @@
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -6988,7 +6988,7 @@
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -7022,7 +7022,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -7083,7 +7083,7 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -7119,7 +7119,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -7213,7 +7213,7 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -7324,7 +7324,7 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -7341,7 +7341,7 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -7418,7 +7418,7 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -7551,7 +7551,7 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -7603,7 +7603,7 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -7622,7 +7622,7 @@
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>Geografi</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -7803,7 +7803,7 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -7840,7 +7840,7 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -7874,7 +7874,7 @@
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -7930,7 +7930,7 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -8002,7 +8002,7 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -8020,7 +8020,7 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -8112,7 +8112,7 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -8184,7 +8184,7 @@
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -8254,7 +8254,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -8271,7 +8271,7 @@
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -8328,7 +8328,7 @@
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -8349,7 +8349,7 @@
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Geografi</t>
         </is>
       </c>
     </row>
@@ -8401,7 +8401,7 @@
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -8460,7 +8460,7 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -8688,7 +8688,7 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -8707,7 +8707,7 @@
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -8745,7 +8745,7 @@
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -8781,7 +8781,7 @@
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -8816,7 +8816,7 @@
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -8978,7 +8978,7 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -8996,7 +8996,7 @@
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -9132,7 +9132,7 @@
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -9244,7 +9244,7 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -9261,7 +9261,7 @@
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -9278,7 +9278,7 @@
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -9404,7 +9404,7 @@
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -9440,7 +9440,7 @@
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -9531,7 +9531,7 @@
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -9604,7 +9604,7 @@
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -9624,7 +9624,7 @@
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -9663,7 +9663,7 @@
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -9715,7 +9715,7 @@
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -9732,7 +9732,7 @@
       </c>
       <c r="C501" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -9786,7 +9786,7 @@
       </c>
       <c r="C504" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -9844,7 +9844,7 @@
       </c>
       <c r="C507" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -9862,7 +9862,7 @@
       </c>
       <c r="C508" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -9879,7 +9879,7 @@
       </c>
       <c r="C509" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -9914,7 +9914,7 @@
       </c>
       <c r="C511" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -9986,7 +9986,7 @@
       </c>
       <c r="C515" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -10092,7 +10092,7 @@
       </c>
       <c r="C521" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -10178,7 +10178,7 @@
       </c>
       <c r="C525" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -10554,7 +10554,7 @@
       </c>
       <c r="C545" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -10593,7 +10593,7 @@
       </c>
       <c r="C547" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -10678,7 +10678,7 @@
       </c>
       <c r="C552" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -10731,7 +10731,7 @@
       </c>
       <c r="C555" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -10749,7 +10749,7 @@
       </c>
       <c r="C556" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -10785,7 +10785,7 @@
       </c>
       <c r="C558" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -10803,7 +10803,7 @@
       </c>
       <c r="C559" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -10897,7 +10897,7 @@
       </c>
       <c r="C564" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -10990,7 +10990,7 @@
       </c>
       <c r="C569" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -11014,7 +11014,7 @@
       </c>
       <c r="C570" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -11055,7 +11055,7 @@
       </c>
       <c r="C572" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -11072,7 +11072,7 @@
       </c>
       <c r="C573" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -11109,7 +11109,7 @@
       </c>
       <c r="C575" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -11127,7 +11127,7 @@
       </c>
       <c r="C576" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -11161,7 +11161,7 @@
       </c>
       <c r="C578" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -11353,7 +11353,7 @@
       </c>
       <c r="C589" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -11460,7 +11460,7 @@
       </c>
       <c r="C593" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -11514,7 +11514,7 @@
       </c>
       <c r="C596" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -11569,7 +11569,7 @@
       </c>
       <c r="C599" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -11601,7 +11601,7 @@
       </c>
       <c r="C600" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -11769,7 +11769,7 @@
       </c>
       <c r="C609" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -11822,7 +11822,7 @@
       </c>
       <c r="C612" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -11856,7 +11856,7 @@
       </c>
       <c r="C614" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -11873,7 +11873,7 @@
       </c>
       <c r="C615" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -11936,7 +11936,7 @@
       </c>
       <c r="C618" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -11956,7 +11956,7 @@
       </c>
       <c r="C619" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -11973,7 +11973,7 @@
       </c>
       <c r="C620" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -12026,7 +12026,7 @@
       </c>
       <c r="C623" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -12043,7 +12043,7 @@
       </c>
       <c r="C624" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -12060,7 +12060,7 @@
       </c>
       <c r="C625" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -12098,7 +12098,7 @@
       </c>
       <c r="C627" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -12244,7 +12244,7 @@
       </c>
       <c r="C635" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -12261,7 +12261,7 @@
       </c>
       <c r="C636" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -12413,7 +12413,7 @@
       </c>
       <c r="C644" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -12506,7 +12506,7 @@
       </c>
       <c r="C649" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -12523,7 +12523,7 @@
       </c>
       <c r="C650" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -12560,7 +12560,7 @@
       </c>
       <c r="C652" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -12577,7 +12577,7 @@
       </c>
       <c r="C653" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -12614,7 +12614,7 @@
       </c>
       <c r="C655" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -12633,7 +12633,7 @@
       </c>
       <c r="C656" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -12705,7 +12705,7 @@
       </c>
       <c r="C659" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -12832,7 +12832,7 @@
       </c>
       <c r="C666" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -13094,7 +13094,7 @@
       </c>
       <c r="C680" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="C686" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -13226,7 +13226,7 @@
       </c>
       <c r="C687" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -13243,7 +13243,7 @@
       </c>
       <c r="C688" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -13316,7 +13316,7 @@
       </c>
       <c r="C692" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -13353,7 +13353,7 @@
       </c>
       <c r="C694" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -13408,7 +13408,7 @@
       </c>
       <c r="C697" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -13480,7 +13480,7 @@
       </c>
       <c r="C701" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -13575,7 +13575,7 @@
       </c>
       <c r="C706" t="inlineStr">
         <is>
-          <t>Geografi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -13593,7 +13593,7 @@
       </c>
       <c r="C707" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -13610,7 +13610,7 @@
       </c>
       <c r="C708" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -13627,7 +13627,7 @@
       </c>
       <c r="C709" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -13679,7 +13679,7 @@
       </c>
       <c r="C712" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -13715,7 +13715,7 @@
       </c>
       <c r="C714" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -13732,7 +13732,7 @@
       </c>
       <c r="C715" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -13755,7 +13755,7 @@
       </c>
       <c r="C716" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -13791,7 +13791,7 @@
       </c>
       <c r="C718" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -13878,7 +13878,7 @@
       </c>
       <c r="C723" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -13967,7 +13967,7 @@
       </c>
       <c r="C728" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -14039,7 +14039,7 @@
       </c>
       <c r="C732" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -14275,7 +14275,7 @@
       </c>
       <c r="C745" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -14360,7 +14360,7 @@
       </c>
       <c r="C750" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -14412,7 +14412,7 @@
       </c>
       <c r="C753" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -14500,7 +14500,7 @@
       </c>
       <c r="C758" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -14534,7 +14534,7 @@
       </c>
       <c r="C760" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -14629,7 +14629,7 @@
       </c>
       <c r="C765" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -14757,7 +14757,7 @@
       </c>
       <c r="C772" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -14777,7 +14777,7 @@
       </c>
       <c r="C773" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -14794,7 +14794,7 @@
       </c>
       <c r="C774" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -14922,7 +14922,7 @@
       </c>
       <c r="C781" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -14975,7 +14975,7 @@
       </c>
       <c r="C784" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -15009,7 +15009,7 @@
       </c>
       <c r="C786" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -15048,7 +15048,7 @@
       </c>
       <c r="C788" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Geografi</t>
         </is>
       </c>
     </row>
@@ -15085,7 +15085,7 @@
       </c>
       <c r="C790" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -15172,7 +15172,7 @@
       </c>
       <c r="C794" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -15243,7 +15243,7 @@
       </c>
       <c r="C798" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -15280,7 +15280,7 @@
       </c>
       <c r="C800" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -15336,7 +15336,7 @@
       </c>
       <c r="C803" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -15391,7 +15391,7 @@
       </c>
       <c r="C806" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -15425,7 +15425,7 @@
       </c>
       <c r="C808" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -15442,7 +15442,7 @@
       </c>
       <c r="C809" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -15533,7 +15533,7 @@
       </c>
       <c r="C814" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -15596,7 +15596,7 @@
       </c>
       <c r="C817" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -15633,7 +15633,7 @@
       </c>
       <c r="C819" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -15687,7 +15687,7 @@
       </c>
       <c r="C822" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -15707,7 +15707,7 @@
       </c>
       <c r="C823" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -15758,7 +15758,7 @@
       </c>
       <c r="C826" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -15868,7 +15868,7 @@
       </c>
       <c r="C832" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -15983,7 +15983,7 @@
       </c>
       <c r="C838" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -16109,7 +16109,7 @@
       </c>
       <c r="C845" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -16126,7 +16126,7 @@
       </c>
       <c r="C846" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -16145,7 +16145,7 @@
       </c>
       <c r="C847" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -16201,7 +16201,7 @@
       </c>
       <c r="C850" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -16312,7 +16312,7 @@
       </c>
       <c r="C856" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -16421,7 +16421,7 @@
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -16456,7 +16456,7 @@
       </c>
       <c r="C864" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -16473,7 +16473,7 @@
       </c>
       <c r="C865" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -16524,7 +16524,7 @@
       </c>
       <c r="C868" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -16541,7 +16541,7 @@
       </c>
       <c r="C869" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -16578,7 +16578,7 @@
       </c>
       <c r="C871" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -16595,7 +16595,7 @@
       </c>
       <c r="C872" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -16616,7 +16616,7 @@
       </c>
       <c r="C873" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -17029,7 +17029,7 @@
       </c>
       <c r="C894" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -17047,7 +17047,7 @@
       </c>
       <c r="C895" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -17100,7 +17100,7 @@
       </c>
       <c r="C898" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Geografi</t>
         </is>
       </c>
     </row>
@@ -17172,7 +17172,7 @@
       </c>
       <c r="C902" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -17207,7 +17207,7 @@
       </c>
       <c r="C904" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -17328,7 +17328,7 @@
       </c>
       <c r="C910" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -17362,7 +17362,7 @@
       </c>
       <c r="C912" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -17402,7 +17402,7 @@
       </c>
       <c r="C914" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -17455,7 +17455,7 @@
       </c>
       <c r="C917" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -17508,7 +17508,7 @@
       </c>
       <c r="C920" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -17564,7 +17564,7 @@
       </c>
       <c r="C923" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -17581,7 +17581,7 @@
       </c>
       <c r="C924" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -17599,7 +17599,7 @@
       </c>
       <c r="C925" t="inlineStr">
         <is>
-          <t>Pertahanan dan Keamanan</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -17634,7 +17634,7 @@
       </c>
       <c r="C927" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -17706,7 +17706,7 @@
       </c>
       <c r="C931" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -17815,7 +17815,7 @@
       </c>
       <c r="C937" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -17833,7 +17833,7 @@
       </c>
       <c r="C938" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -17898,7 +17898,7 @@
       </c>
       <c r="C941" t="inlineStr">
         <is>
-          <t>Ideologi</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -17919,7 +17919,7 @@
       </c>
       <c r="C942" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -18015,7 +18015,7 @@
       </c>
       <c r="C947" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -18126,7 +18126,7 @@
       </c>
       <c r="C953" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -18214,7 +18214,7 @@
       </c>
       <c r="C958" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -18249,7 +18249,7 @@
       </c>
       <c r="C960" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -18270,7 +18270,7 @@
       </c>
       <c r="C961" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -18287,7 +18287,7 @@
       </c>
       <c r="C962" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -18325,7 +18325,7 @@
       </c>
       <c r="C964" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ekonomi</t>
         </is>
       </c>
     </row>
@@ -18411,7 +18411,7 @@
       </c>
       <c r="C968" t="inlineStr">
         <is>
-          <t>Sosial Budaya</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -18481,7 +18481,7 @@
       </c>
       <c r="C972" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Geografi</t>
         </is>
       </c>
     </row>
@@ -18501,7 +18501,7 @@
       </c>
       <c r="C973" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Ideologi</t>
         </is>
       </c>
     </row>
@@ -18519,7 +18519,7 @@
       </c>
       <c r="C974" t="inlineStr">
         <is>
-          <t>Sumber Daya Alam</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -18588,7 +18588,7 @@
       </c>
       <c r="C978" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -18611,7 +18611,7 @@
       </c>
       <c r="C979" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sumber Daya Alam</t>
         </is>
       </c>
     </row>
@@ -18630,7 +18630,7 @@
       </c>
       <c r="C980" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Pertahanan dan Keamanan</t>
         </is>
       </c>
     </row>
@@ -18706,7 +18706,7 @@
       </c>
       <c r="C984" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -18792,7 +18792,7 @@
       </c>
       <c r="C988" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Sosial Budaya</t>
         </is>
       </c>
     </row>
@@ -18848,7 +18848,7 @@
       </c>
       <c r="C991" t="inlineStr">
         <is>
-          <t>Demografi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>
@@ -18982,7 +18982,7 @@
       </c>
       <c r="C998" t="inlineStr">
         <is>
-          <t>Politik</t>
+          <t>Demografi</t>
         </is>
       </c>
     </row>
@@ -19033,7 +19033,7 @@
       </c>
       <c r="C1001" t="inlineStr">
         <is>
-          <t>Ekonomi</t>
+          <t>Politik</t>
         </is>
       </c>
     </row>

</xml_diff>